<commit_message>
update table view and make it show in debug view.
</commit_message>
<xml_diff>
--- a/IntranetPortal/IntranetPortal/App_Data/underwriter.xlsx
+++ b/IntranetPortal/IntranetPortal/App_Data/underwriter.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Data Input" sheetId="4" r:id="rId1"/>
     <sheet name="Flip Sheets" sheetId="3" r:id="rId2"/>
     <sheet name="Rental Model" sheetId="7" r:id="rId3"/>
-    <sheet name="Tables" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="Tables" sheetId="2" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="200">
   <si>
     <t>Property Address:</t>
   </si>
@@ -857,7 +857,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1166,6 +1166,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1181,7 +1218,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="356">
+  <cellXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1880,10 +1917,6 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1908,22 +1941,10 @@
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1934,10 +1955,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -2066,26 +2083,10 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -2110,14 +2111,6 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
@@ -2152,6 +2145,46 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -2212,35 +2245,35 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
@@ -2650,7 +2683,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,17 +2753,17 @@
       <c r="B3" s="198" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="250"/>
+      <c r="C3" s="246"/>
       <c r="D3" s="191"/>
-      <c r="E3" s="252" t="s">
+      <c r="E3" s="248" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="253"/>
+      <c r="F3" s="310"/>
       <c r="G3" s="194"/>
       <c r="H3" s="198" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="304"/>
+      <c r="I3" s="310"/>
       <c r="J3" s="164"/>
       <c r="K3" s="196" t="s">
         <v>142</v>
@@ -2751,12 +2784,12 @@
       <c r="E4" s="199" t="s">
         <v>145</v>
       </c>
-      <c r="F4" s="246"/>
+      <c r="F4" s="296"/>
       <c r="G4" s="194"/>
       <c r="H4" s="200" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="305"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="164"/>
       <c r="K4" s="164"/>
       <c r="L4" s="165"/>
@@ -2772,17 +2805,19 @@
       <c r="E5" s="200" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="240"/>
+      <c r="F5" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G5" s="194"/>
       <c r="H5" s="200" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="305"/>
+      <c r="I5" s="312"/>
       <c r="J5" s="164"/>
-      <c r="K5" s="318" t="s">
+      <c r="K5" s="317" t="s">
         <v>173</v>
       </c>
-      <c r="L5" s="319"/>
+      <c r="L5" s="318"/>
       <c r="M5" s="164"/>
       <c r="O5" s="221"/>
     </row>
@@ -2791,22 +2826,24 @@
       <c r="B6" s="201" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="251"/>
+      <c r="C6" s="247"/>
       <c r="D6" s="191"/>
       <c r="E6" s="200" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="240"/>
+      <c r="F6" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G6" s="194"/>
       <c r="H6" s="200" t="s">
         <v>196</v>
       </c>
-      <c r="I6" s="305"/>
+      <c r="I6" s="312"/>
       <c r="J6" s="164"/>
-      <c r="K6" s="265" t="s">
+      <c r="K6" s="260" t="s">
         <v>167</v>
       </c>
-      <c r="L6" s="266" t="e">
+      <c r="L6" s="261" t="e">
         <f ca="1">SUM(Tables!B6:B25)</f>
         <v>#VALUE!</v>
       </c>
@@ -2822,17 +2859,19 @@
       <c r="E7" s="200" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="306"/>
+      <c r="F7" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G7" s="194"/>
       <c r="H7" s="200" t="s">
         <v>190</v>
       </c>
-      <c r="I7" s="305"/>
+      <c r="I7" s="312"/>
       <c r="J7" s="164"/>
-      <c r="K7" s="267" t="s">
+      <c r="K7" s="262" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="268" t="e">
+      <c r="L7" s="263" t="e">
         <f ca="1">'Flip Sheets'!C26</f>
         <v>#VALUE!</v>
       </c>
@@ -2845,20 +2884,22 @@
       </c>
       <c r="C8" s="238"/>
       <c r="D8" s="191"/>
-      <c r="E8" s="255" t="s">
+      <c r="E8" s="250" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="293"/>
+      <c r="F8" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G8" s="194"/>
       <c r="H8" s="200" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="305"/>
+      <c r="I8" s="312"/>
       <c r="J8" s="164"/>
-      <c r="K8" s="267" t="s">
+      <c r="K8" s="262" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="268" t="e">
+      <c r="L8" s="263" t="e">
         <f ca="1">'Flip Sheets'!H23</f>
         <v>#VALUE!</v>
       </c>
@@ -2866,25 +2907,27 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="188"/>
-      <c r="B9" s="255" t="s">
+      <c r="B9" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="293"/>
+      <c r="C9" s="288"/>
       <c r="D9" s="191"/>
       <c r="E9" s="200" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="240"/>
+      <c r="F9" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G9" s="194"/>
       <c r="H9" s="200" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="305"/>
+      <c r="I9" s="312"/>
       <c r="J9" s="164"/>
-      <c r="K9" s="267" t="s">
+      <c r="K9" s="262" t="s">
         <v>171</v>
       </c>
-      <c r="L9" s="269" t="e">
+      <c r="L9" s="264" t="e">
         <f ca="1">'Flip Sheets'!F26</f>
         <v>#VALUE!</v>
       </c>
@@ -2892,25 +2935,27 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="188"/>
-      <c r="B10" s="255" t="s">
+      <c r="B10" s="250" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="293"/>
+      <c r="C10" s="288"/>
       <c r="D10" s="191"/>
       <c r="E10" s="200" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="240"/>
+      <c r="F10" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G10" s="194"/>
       <c r="H10" s="200" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="305"/>
+      <c r="I10" s="312"/>
       <c r="J10" s="164"/>
-      <c r="K10" s="270" t="s">
+      <c r="K10" s="265" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="271" t="e">
+      <c r="L10" s="266" t="e">
         <f ca="1">'Flip Sheets'!H25</f>
         <v>#VALUE!</v>
       </c>
@@ -2921,17 +2966,19 @@
       <c r="B11" s="200" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="294"/>
+      <c r="C11" s="289"/>
       <c r="D11" s="191"/>
       <c r="E11" s="200" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="240"/>
+      <c r="F11" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G11" s="194"/>
-      <c r="H11" s="254" t="s">
+      <c r="H11" s="249" t="s">
         <v>185</v>
       </c>
-      <c r="I11" s="305"/>
+      <c r="I11" s="312"/>
       <c r="J11" s="164"/>
       <c r="K11" s="157"/>
       <c r="L11" s="158"/>
@@ -2942,22 +2989,22 @@
       <c r="B12" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="303"/>
+      <c r="C12" s="294"/>
       <c r="D12" s="191"/>
       <c r="E12" s="200" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="240"/>
+      <c r="F12" s="239"/>
       <c r="G12" s="194"/>
       <c r="H12" s="200" t="s">
         <v>189</v>
       </c>
-      <c r="I12" s="305"/>
+      <c r="I12" s="296"/>
       <c r="J12" s="164"/>
-      <c r="K12" s="320" t="s">
+      <c r="K12" s="319" t="s">
         <v>172</v>
       </c>
-      <c r="L12" s="321"/>
+      <c r="L12" s="320"/>
       <c r="M12" s="164"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2965,7 +3012,7 @@
       <c r="B13" s="200" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="240"/>
+      <c r="C13" s="239"/>
       <c r="D13" s="191"/>
       <c r="E13" s="201" t="s">
         <v>147</v>
@@ -2975,7 +3022,9 @@
       <c r="H13" s="200" t="s">
         <v>186</v>
       </c>
-      <c r="I13" s="240"/>
+      <c r="I13" s="315" t="s">
+        <v>67</v>
+      </c>
       <c r="J13" s="164"/>
       <c r="K13" s="203" t="s">
         <v>167</v>
@@ -2991,19 +3040,19 @@
       <c r="B14" s="199" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="240" t="s">
+      <c r="C14" s="239" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="207"/>
       <c r="E14" s="200" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="247"/>
+      <c r="F14" s="245"/>
       <c r="G14" s="194"/>
       <c r="H14" s="200" t="s">
         <v>188</v>
       </c>
-      <c r="I14" s="305"/>
+      <c r="I14" s="312"/>
       <c r="J14" s="164"/>
       <c r="K14" s="159" t="s">
         <v>8</v>
@@ -3019,17 +3068,17 @@
       <c r="B15" s="202" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="241"/>
+      <c r="C15" s="240"/>
       <c r="D15" s="207"/>
       <c r="E15" s="200" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="247"/>
+      <c r="F15" s="245"/>
       <c r="G15" s="194"/>
-      <c r="H15" s="254" t="s">
+      <c r="H15" s="249" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="306"/>
+      <c r="I15" s="296"/>
       <c r="J15" s="164"/>
       <c r="K15" s="159" t="s">
         <v>17</v>
@@ -3048,12 +3097,14 @@
       <c r="E16" s="209" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="306"/>
+      <c r="F16" s="307"/>
       <c r="G16" s="194"/>
       <c r="H16" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="I16" s="240"/>
+      <c r="I16" s="315" t="s">
+        <v>67</v>
+      </c>
       <c r="J16" s="164"/>
       <c r="K16" s="159" t="s">
         <v>171</v>
@@ -3074,12 +3125,12 @@
       <c r="E17" s="200" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="248"/>
+      <c r="F17" s="309"/>
       <c r="G17" s="194"/>
       <c r="H17" s="200" t="s">
         <v>102</v>
       </c>
-      <c r="I17" s="305"/>
+      <c r="I17" s="312"/>
       <c r="J17" s="164"/>
       <c r="K17" s="160" t="s">
         <v>143</v>
@@ -3100,12 +3151,12 @@
       <c r="E18" s="200" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="239"/>
+      <c r="F18" s="296"/>
       <c r="G18" s="164"/>
       <c r="H18" s="208" t="s">
         <v>135</v>
       </c>
-      <c r="I18" s="307"/>
+      <c r="I18" s="316"/>
       <c r="J18" s="164"/>
       <c r="K18" s="212"/>
       <c r="L18" s="165"/>
@@ -3113,24 +3164,23 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="188"/>
-      <c r="B19" s="255" t="s">
+      <c r="B19" s="250" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="293" t="str">
-        <f>IF(OR('Data Input'!C14="Yes",'Data Input'!C15&gt;0)*AND('Data Input'!F9&lt;&gt;"Yes",'Data Input'!F10&lt;&gt;"Yes",'Data Input'!F11&lt;&gt;"Yes",'Data Input'!C20&lt;&gt;"",'Data Input'!C20&gt;0),"Yes","No")</f>
-        <v>No</v>
+      <c r="C19" s="311" t="s">
+        <v>67</v>
       </c>
       <c r="D19" s="191"/>
       <c r="E19" s="200" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="248"/>
+      <c r="F19" s="309"/>
       <c r="G19" s="188"/>
       <c r="J19" s="164"/>
-      <c r="K19" s="322" t="s">
+      <c r="K19" s="321" t="s">
         <v>194</v>
       </c>
-      <c r="L19" s="323"/>
+      <c r="L19" s="322"/>
       <c r="M19" s="164"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3143,15 +3193,15 @@
       <c r="E20" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="249"/>
+      <c r="F20" s="313"/>
       <c r="G20" s="188"/>
       <c r="H20" s="164"/>
       <c r="I20" s="164"/>
       <c r="J20" s="164"/>
-      <c r="K20" s="272" t="s">
+      <c r="K20" s="267" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="291" t="e">
+      <c r="L20" s="286" t="e">
         <f ca="1">'Flip Sheets'!C33</f>
         <v>#VALUE!</v>
       </c>
@@ -3159,18 +3209,18 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="188"/>
-      <c r="B21" s="255" t="s">
+      <c r="B21" s="250" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="297">
-        <v>0.75</v>
+      <c r="C21" s="290">
+        <v>0</v>
       </c>
       <c r="D21" s="194"/>
       <c r="J21" s="164"/>
-      <c r="K21" s="274" t="s">
+      <c r="K21" s="269" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="273" t="e">
+      <c r="L21" s="268" t="e">
         <f ca="1">'Flip Sheets'!F33</f>
         <v>#VALUE!</v>
       </c>
@@ -3181,7 +3231,7 @@
       <c r="B22" s="209" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="298"/>
+      <c r="C22" s="312"/>
       <c r="D22" s="194"/>
       <c r="E22" s="215" t="s">
         <v>61</v>
@@ -3191,10 +3241,10 @@
       <c r="H22" s="217"/>
       <c r="I22" s="218"/>
       <c r="J22" s="164"/>
-      <c r="K22" s="275" t="s">
+      <c r="K22" s="270" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="292" t="e">
+      <c r="L22" s="287" t="e">
         <f ca="1">'Flip Sheets'!H33</f>
         <v>#VALUE!</v>
       </c>
@@ -3205,16 +3255,16 @@
       <c r="B23" s="211" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="249"/>
+      <c r="C23" s="313"/>
       <c r="D23" s="194"/>
-      <c r="E23" s="324"/>
-      <c r="F23" s="325"/>
-      <c r="G23" s="325"/>
-      <c r="H23" s="325"/>
-      <c r="I23" s="326"/>
+      <c r="E23" s="323"/>
+      <c r="F23" s="324"/>
+      <c r="G23" s="324"/>
+      <c r="H23" s="324"/>
+      <c r="I23" s="325"/>
       <c r="J23" s="164"/>
-      <c r="K23" s="289"/>
-      <c r="L23" s="290"/>
+      <c r="K23" s="284"/>
+      <c r="L23" s="285"/>
       <c r="M23" s="164"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3222,16 +3272,16 @@
       <c r="B24" s="164"/>
       <c r="C24" s="213"/>
       <c r="D24" s="194"/>
-      <c r="E24" s="327"/>
-      <c r="F24" s="328"/>
-      <c r="G24" s="328"/>
-      <c r="H24" s="328"/>
-      <c r="I24" s="329"/>
+      <c r="E24" s="326"/>
+      <c r="F24" s="327"/>
+      <c r="G24" s="327"/>
+      <c r="H24" s="327"/>
+      <c r="I24" s="328"/>
       <c r="J24" s="164"/>
-      <c r="K24" s="316" t="s">
+      <c r="K24" s="305" t="s">
         <v>178</v>
       </c>
-      <c r="L24" s="317" t="e">
+      <c r="L24" s="306" t="e">
         <f ca="1">Tables!J22-Tables!J29</f>
         <v>#VALUE!</v>
       </c>
@@ -3244,11 +3294,11 @@
       </c>
       <c r="C25" s="214"/>
       <c r="D25" s="194"/>
-      <c r="E25" s="327"/>
-      <c r="F25" s="328"/>
-      <c r="G25" s="328"/>
-      <c r="H25" s="328"/>
-      <c r="I25" s="329"/>
+      <c r="E25" s="326"/>
+      <c r="F25" s="327"/>
+      <c r="G25" s="327"/>
+      <c r="H25" s="327"/>
+      <c r="I25" s="328"/>
       <c r="J25" s="164"/>
       <c r="K25" s="164"/>
       <c r="L25" s="165"/>
@@ -3256,31 +3306,31 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="188"/>
-      <c r="B26" s="276" t="s">
+      <c r="B26" s="271" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="299"/>
+      <c r="C26" s="295"/>
       <c r="D26" s="194"/>
-      <c r="E26" s="327"/>
-      <c r="F26" s="328"/>
-      <c r="G26" s="328"/>
-      <c r="H26" s="328"/>
-      <c r="I26" s="329"/>
+      <c r="E26" s="326"/>
+      <c r="F26" s="327"/>
+      <c r="G26" s="327"/>
+      <c r="H26" s="327"/>
+      <c r="I26" s="328"/>
       <c r="J26" s="164"/>
       <c r="M26" s="164"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="188"/>
-      <c r="B27" s="200" t="s">
+      <c r="B27" s="308" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="296"/>
+      <c r="C27" s="314"/>
       <c r="D27" s="194"/>
-      <c r="E27" s="327"/>
-      <c r="F27" s="328"/>
-      <c r="G27" s="328"/>
-      <c r="H27" s="328"/>
-      <c r="I27" s="329"/>
+      <c r="E27" s="326"/>
+      <c r="F27" s="327"/>
+      <c r="G27" s="327"/>
+      <c r="H27" s="327"/>
+      <c r="I27" s="328"/>
       <c r="J27" s="164"/>
       <c r="K27" s="219"/>
       <c r="L27" s="220"/>
@@ -3293,27 +3343,29 @@
       </c>
       <c r="C28" s="296"/>
       <c r="D28" s="194"/>
-      <c r="E28" s="327"/>
-      <c r="F28" s="328"/>
-      <c r="G28" s="328"/>
-      <c r="H28" s="328"/>
-      <c r="I28" s="329"/>
+      <c r="E28" s="326"/>
+      <c r="F28" s="327"/>
+      <c r="G28" s="327"/>
+      <c r="H28" s="327"/>
+      <c r="I28" s="328"/>
       <c r="J28" s="164"/>
       <c r="K28" s="219"/>
       <c r="M28" s="164"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="188"/>
-      <c r="B29" s="255" t="s">
+      <c r="B29" s="250" t="s">
         <v>195</v>
       </c>
-      <c r="C29" s="240"/>
+      <c r="C29" s="237" t="s">
+        <v>67</v>
+      </c>
       <c r="D29" s="194"/>
-      <c r="E29" s="327"/>
-      <c r="F29" s="328"/>
-      <c r="G29" s="328"/>
-      <c r="H29" s="328"/>
-      <c r="I29" s="329"/>
+      <c r="E29" s="326"/>
+      <c r="F29" s="327"/>
+      <c r="G29" s="327"/>
+      <c r="H29" s="327"/>
+      <c r="I29" s="328"/>
       <c r="J29" s="164"/>
       <c r="K29" s="219"/>
       <c r="L29" s="222"/>
@@ -3324,15 +3376,13 @@
       <c r="B30" s="200" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="300">
-        <v>6</v>
-      </c>
+      <c r="C30" s="291"/>
       <c r="D30" s="194"/>
-      <c r="E30" s="327"/>
-      <c r="F30" s="328"/>
-      <c r="G30" s="328"/>
-      <c r="H30" s="328"/>
-      <c r="I30" s="329"/>
+      <c r="E30" s="326"/>
+      <c r="F30" s="327"/>
+      <c r="G30" s="327"/>
+      <c r="H30" s="327"/>
+      <c r="I30" s="328"/>
       <c r="J30" s="164"/>
       <c r="K30" s="219"/>
       <c r="L30" s="220"/>
@@ -3343,15 +3393,15 @@
       <c r="B31" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="301">
+      <c r="C31" s="292">
         <v>0.05</v>
       </c>
       <c r="D31" s="194"/>
-      <c r="E31" s="327"/>
-      <c r="F31" s="328"/>
-      <c r="G31" s="328"/>
-      <c r="H31" s="328"/>
-      <c r="I31" s="329"/>
+      <c r="E31" s="326"/>
+      <c r="F31" s="327"/>
+      <c r="G31" s="327"/>
+      <c r="H31" s="327"/>
+      <c r="I31" s="328"/>
       <c r="J31" s="164"/>
       <c r="K31" s="219"/>
       <c r="L31" s="220"/>
@@ -3362,15 +3412,15 @@
       <c r="B32" s="208" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="302">
+      <c r="C32" s="293">
         <v>0.35</v>
       </c>
       <c r="D32" s="194"/>
-      <c r="E32" s="330"/>
-      <c r="F32" s="331"/>
-      <c r="G32" s="331"/>
-      <c r="H32" s="331"/>
-      <c r="I32" s="332"/>
+      <c r="E32" s="329"/>
+      <c r="F32" s="330"/>
+      <c r="G32" s="330"/>
+      <c r="H32" s="330"/>
+      <c r="I32" s="331"/>
       <c r="J32" s="164"/>
       <c r="K32" s="219"/>
       <c r="L32" s="220"/>
@@ -3387,7 +3437,7 @@
       <c r="M34" s="147"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="plRIxWnjwlPp/Gyc+sZf1BpkoQrRT8zKRaBxPrgANaelZPQYIe+JOeyFqmLYBHpYVxPB2VEv31DyQqIH6h63Mg==" saltValue="QXZ8wZvYmKXkCUN0nfdsbA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <dataConsolidate/>
   <mergeCells count="4">
     <mergeCell ref="K5:L5"/>
@@ -3400,7 +3450,7 @@
     <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F20 F18 C27:C28 I14 C12 C23 I17 C20 C18 C30 I3:I12">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18 I17 C22:C23 I3:I12 C12 C20 I14:I15 C18 F3:F4 C30 F20 C26:C28">
       <formula1>-1000000</formula1>
     </dataValidation>
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C15">
@@ -3418,48 +3468,42 @@
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$8</xm:f>
           </x14:formula1>
           <xm:sqref>C13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F6</xm:sqref>
+          <xm:sqref>C29 F5:F11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Tables!$J$2:$J$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
           <xm:sqref>I16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
           <xm:sqref>C14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
           <xm:sqref>I13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F9:F11</xm:sqref>
+          <xm:sqref>C19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3472,7 +3516,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I41"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3505,13 +3549,13 @@
       <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="335">
+      <c r="C2" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D2" s="335"/>
-      <c r="E2" s="335"/>
-      <c r="F2" s="336"/>
+      <c r="D2" s="332"/>
+      <c r="E2" s="332"/>
+      <c r="F2" s="333"/>
       <c r="G2" s="43"/>
       <c r="H2" s="44" t="s">
         <v>44</v>
@@ -3523,8 +3567,8 @@
       <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="311">
-        <f>'Data Input'!C4</f>
+      <c r="C3" s="300">
+        <f>'Data Input'!C5</f>
         <v>0</v>
       </c>
       <c r="D3" s="25"/>
@@ -3537,22 +3581,22 @@
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="84">
-        <f>'Data Input'!C28</f>
+        <f>'Data Input'!C30</f>
         <v>0</v>
       </c>
       <c r="I3" s="39"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39"/>
-      <c r="B4" s="339" t="s">
+      <c r="B4" s="336" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="340"/>
+      <c r="C4" s="337"/>
       <c r="D4" s="48"/>
-      <c r="E4" s="339" t="s">
+      <c r="E4" s="336" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="340"/>
+      <c r="F4" s="337"/>
       <c r="G4" s="49"/>
       <c r="H4" s="50" t="s">
         <v>42</v>
@@ -3745,13 +3789,13 @@
       <c r="B15" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="335">
+      <c r="C15" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D15" s="335"/>
-      <c r="E15" s="335"/>
-      <c r="F15" s="336"/>
+      <c r="D15" s="332"/>
+      <c r="E15" s="332"/>
+      <c r="F15" s="333"/>
       <c r="G15" s="43"/>
       <c r="H15" s="138" t="s">
         <v>44</v>
@@ -3763,7 +3807,7 @@
       <c r="B16" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="311">
+      <c r="C16" s="300">
         <f>'Data Input'!C4</f>
         <v>0</v>
       </c>
@@ -3777,22 +3821,22 @@
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="139">
-        <f>'Data Input'!C28</f>
+        <f>'Data Input'!C30</f>
         <v>0</v>
       </c>
       <c r="I16" s="39"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39"/>
-      <c r="B17" s="337" t="s">
+      <c r="B17" s="334" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="338"/>
+      <c r="C17" s="335"/>
       <c r="D17" s="48"/>
-      <c r="E17" s="337" t="s">
+      <c r="E17" s="334" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="338"/>
+      <c r="F17" s="335"/>
       <c r="G17" s="59"/>
       <c r="H17" s="60" t="s">
         <v>62</v>
@@ -4026,13 +4070,13 @@
       <c r="B30" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="335">
+      <c r="C30" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D30" s="335"/>
-      <c r="E30" s="335"/>
-      <c r="F30" s="336"/>
+      <c r="D30" s="332"/>
+      <c r="E30" s="332"/>
+      <c r="F30" s="333"/>
       <c r="G30" s="43"/>
       <c r="H30" s="64"/>
       <c r="I30" s="39"/>
@@ -4042,7 +4086,7 @@
       <c r="B31" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="311">
+      <c r="C31" s="300">
         <f>'Data Input'!C4</f>
         <v>0</v>
       </c>
@@ -4060,15 +4104,15 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39"/>
-      <c r="B32" s="333" t="s">
+      <c r="B32" s="338" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="334"/>
+      <c r="C32" s="339"/>
       <c r="D32" s="48"/>
-      <c r="E32" s="333" t="s">
+      <c r="E32" s="338" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="334"/>
+      <c r="F32" s="339"/>
       <c r="G32" s="49"/>
       <c r="H32" s="67" t="s">
         <v>40</v>
@@ -4112,15 +4156,15 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="39"/>
-      <c r="B35" s="333" t="s">
+      <c r="B35" s="338" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="334"/>
+      <c r="C35" s="339"/>
       <c r="D35" s="48"/>
-      <c r="E35" s="333" t="s">
+      <c r="E35" s="338" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="334"/>
+      <c r="F35" s="339"/>
       <c r="G35" s="49"/>
       <c r="H35" s="67" t="s">
         <v>54</v>
@@ -4254,19 +4298,19 @@
       <c r="I41" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6AkjZXVSFB0ziVOXcrpeHhh/HLATkbQVxrQZuEWcVLXwzsunA6rRgTpZldJaFHDBfmDujtzSf7DiifC4AGzaPQ==" saltValue="N+SbVL6VG7pgvFTwtEdyCA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="11">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="E38:E39">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
@@ -4284,7 +4328,7 @@
   <dimension ref="A1:O399"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4326,14 +4370,14 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="312" t="s">
+      <c r="B2" s="301" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="313"/>
-      <c r="E2" s="341" t="s">
+      <c r="C2" s="302"/>
+      <c r="E2" s="340" t="s">
         <v>197</v>
       </c>
-      <c r="F2" s="342"/>
+      <c r="F2" s="341"/>
       <c r="J2" s="163"/>
       <c r="K2" s="164">
         <v>1</v>
@@ -4351,14 +4395,16 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="314" t="s">
+      <c r="B3" s="303" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="242"/>
-      <c r="E3" s="281" t="s">
+      <c r="C3" s="241">
+        <v>0</v>
+      </c>
+      <c r="E3" s="276" t="s">
         <v>198</v>
       </c>
-      <c r="F3" s="287">
+      <c r="F3" s="282">
         <f>C18</f>
         <v>0</v>
       </c>
@@ -4384,16 +4430,16 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="255" t="s">
+      <c r="B4" s="250" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="243" t="s">
+      <c r="C4" s="242" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="283" t="s">
+      <c r="E4" s="278" t="s">
         <v>199</v>
       </c>
-      <c r="F4" s="282">
+      <c r="F4" s="277">
         <f>F20</f>
         <v>-110</v>
       </c>
@@ -4419,14 +4465,16 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="314" t="s">
+      <c r="B5" s="303" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="242"/>
-      <c r="E5" s="283" t="s">
+      <c r="C5" s="241">
+        <v>0</v>
+      </c>
+      <c r="E5" s="278" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="286" t="e">
+      <c r="F5" s="281" t="e">
         <f>H12</f>
         <v>#N/A</v>
       </c>
@@ -4452,16 +4500,18 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="314" t="s">
+      <c r="B6" s="303" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="244"/>
-      <c r="E6" s="283" t="s">
+      <c r="C6" s="243">
+        <v>0</v>
+      </c>
+      <c r="E6" s="278" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="284" t="e">
+      <c r="F6" s="279">
         <f>H14</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J6" s="163"/>
       <c r="K6" s="164">
@@ -4485,14 +4535,16 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="314" t="s">
+      <c r="B7" s="303" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="242"/>
-      <c r="E7" s="285" t="s">
+      <c r="C7" s="241">
+        <v>0</v>
+      </c>
+      <c r="E7" s="280" t="s">
         <v>170</v>
       </c>
-      <c r="F7" s="288" t="e">
+      <c r="F7" s="283" t="e">
         <f>H16</f>
         <v>#N/A</v>
       </c>
@@ -4518,10 +4570,12 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="315" t="s">
+      <c r="B8" s="304" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="245"/>
+      <c r="C8" s="244">
+        <v>0</v>
+      </c>
       <c r="J8" s="163"/>
       <c r="K8" s="164">
         <v>7</v>
@@ -4601,13 +4655,13 @@
       <c r="B11" s="167" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="335">
+      <c r="C11" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D11" s="335"/>
-      <c r="E11" s="335"/>
-      <c r="F11" s="336"/>
+      <c r="D11" s="332"/>
+      <c r="E11" s="332"/>
+      <c r="F11" s="333"/>
       <c r="G11" s="39"/>
       <c r="H11" s="148" t="s">
         <v>165</v>
@@ -4639,11 +4693,11 @@
       <c r="B12" s="168" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="347">
+      <c r="C12" s="346">
         <f>'Rental Model'!C6</f>
         <v>0</v>
       </c>
-      <c r="D12" s="347"/>
+      <c r="D12" s="346"/>
       <c r="E12" s="41" t="s">
         <v>158</v>
       </c>
@@ -4682,11 +4736,11 @@
       <c r="B13" s="170" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="348" t="e">
+      <c r="C13" s="347">
         <f>IF('Rental Model'!C8="",MATCH(1,INDEX(--(O2:O97&gt;F13),0),0),'Rental Model'!C7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D13" s="348"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="347"/>
       <c r="E13" s="171" t="s">
         <v>169</v>
       </c>
@@ -4720,19 +4774,19 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="39"/>
-      <c r="B14" s="343" t="s">
+      <c r="B14" s="342" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="344"/>
+      <c r="C14" s="343"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="345" t="s">
+      <c r="E14" s="344" t="s">
         <v>160</v>
       </c>
-      <c r="F14" s="346"/>
+      <c r="F14" s="345"/>
       <c r="G14" s="39"/>
-      <c r="H14" s="150" t="e">
+      <c r="H14" s="150">
         <f>C13</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="I14" s="39"/>
       <c r="K14" s="164">
@@ -4760,7 +4814,7 @@
       <c r="B15" s="173" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="280">
+      <c r="C15" s="275">
         <f>'Rental Model'!C3</f>
         <v>0</v>
       </c>
@@ -4768,7 +4822,7 @@
       <c r="E15" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="F15" s="280">
+      <c r="F15" s="275">
         <f>'Rental Model'!C7</f>
         <v>0</v>
       </c>
@@ -4802,7 +4856,7 @@
       <c r="B16" s="176" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="280">
+      <c r="C16" s="275">
         <f>'Rental Model'!C5</f>
         <v>0</v>
       </c>
@@ -4886,7 +4940,7 @@
       <c r="B18" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="280">
+      <c r="C18" s="275">
         <f>SUM(C15:C17)</f>
         <v>0</v>
       </c>
@@ -12368,13 +12422,13 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
@@ -12398,19 +12452,19 @@
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="349">
+      <c r="B1" s="348">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="C1" s="350"/>
-      <c r="D1" s="350"/>
-      <c r="E1" s="350"/>
+      <c r="C1" s="349"/>
+      <c r="D1" s="349"/>
+      <c r="E1" s="349"/>
       <c r="F1" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="308">
+      <c r="G1" s="297">
         <f>'Data Input'!C30</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I1" s="90" t="s">
         <v>108</v>
@@ -12418,10 +12472,10 @@
       <c r="J1" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="352" t="s">
+      <c r="L1" s="351" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="353"/>
+      <c r="M1" s="352"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -12444,7 +12498,7 @@
       <c r="F2" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="309">
+      <c r="G2" s="298">
         <f>'Data Input'!C32</f>
         <v>0.35</v>
       </c>
@@ -12453,14 +12507,14 @@
       <c r="L2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="351" t="s">
+      <c r="M2" s="350" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="351"/>
-      <c r="O2" s="354" t="s">
+      <c r="N2" s="350"/>
+      <c r="O2" s="353" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="354"/>
+      <c r="P2" s="353"/>
       <c r="Q2" s="8"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12482,7 +12536,7 @@
       <c r="F3" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="310">
+      <c r="G3" s="299">
         <v>0</v>
       </c>
       <c r="I3" s="92" t="s">
@@ -12495,16 +12549,16 @@
         <f ca="1">Tables!B6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M3" s="355" t="e">
+      <c r="M3" s="354" t="e">
         <f ca="1">IF(Tables!F13&gt;=Tables!B6,Tables!B6,Tables!F13)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N3" s="355"/>
-      <c r="O3" s="355" t="e">
+      <c r="N3" s="354"/>
+      <c r="O3" s="354" t="e">
         <f ca="1">Tables!F13-Tables!M3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P3" s="355"/>
+      <c r="P3" s="354"/>
       <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12556,14 +12610,14 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="261" t="s">
+      <c r="A6" s="256" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="262" t="e">
+      <c r="B6" s="257" t="e">
         <f ca="1">(F6-SUM(B7:B19,B21:B25,B28:B29,B31:B32,B34:B36,F7:F11)-(SUM(B7:B19,B21:B25,B28:B29,B31:B32,B34:B36)*G2))/((G2*1.0058)+1.0058)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C6" s="256">
+      <c r="C6" s="251">
         <v>1</v>
       </c>
       <c r="E6" s="101" t="s">
@@ -12601,11 +12655,11 @@
       <c r="A7" s="200" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="263">
+      <c r="B7" s="258">
         <f>'Data Input'!I3*(1+(C7*'Data Input'!C30))</f>
         <v>0</v>
       </c>
-      <c r="C7" s="257">
+      <c r="C7" s="252">
         <f>0.09/12</f>
         <v>7.4999999999999997E-3</v>
       </c>
@@ -12643,11 +12697,11 @@
       <c r="A8" s="200" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="263">
+      <c r="B8" s="258">
         <f>'Data Input'!I4*C8</f>
         <v>0</v>
       </c>
-      <c r="C8" s="258">
+      <c r="C8" s="253">
         <v>1</v>
       </c>
       <c r="E8" s="101" t="s">
@@ -12685,11 +12739,11 @@
       <c r="A9" s="200" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="263">
+      <c r="B9" s="258">
         <f>'Data Input'!I5*C9</f>
         <v>0</v>
       </c>
-      <c r="C9" s="258">
+      <c r="C9" s="253">
         <v>1</v>
       </c>
       <c r="E9" s="101" t="s">
@@ -12725,11 +12779,11 @@
       <c r="A10" s="200" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="263">
+      <c r="B10" s="258">
         <f>'Data Input'!I6*C10</f>
         <v>0</v>
       </c>
-      <c r="C10" s="258">
+      <c r="C10" s="253">
         <v>1</v>
       </c>
       <c r="E10" s="101" t="s">
@@ -12767,11 +12821,11 @@
       <c r="A11" s="200" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="263">
+      <c r="B11" s="258">
         <f>'Data Input'!I7*C11</f>
         <v>0</v>
       </c>
-      <c r="C11" s="258">
+      <c r="C11" s="253">
         <v>1</v>
       </c>
       <c r="E11" s="101" t="s">
@@ -12812,11 +12866,11 @@
       <c r="A12" s="200" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="263">
+      <c r="B12" s="258">
         <f>'Data Input'!I8*C12</f>
         <v>0</v>
       </c>
-      <c r="C12" s="258">
+      <c r="C12" s="253">
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -12848,11 +12902,11 @@
       <c r="A13" s="200" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="263">
+      <c r="B13" s="258">
         <f>'Data Input'!I9*C13</f>
         <v>0</v>
       </c>
-      <c r="C13" s="258">
+      <c r="C13" s="253">
         <v>0.15</v>
       </c>
       <c r="E13" s="101" t="s">
@@ -12883,11 +12937,11 @@
       <c r="A14" s="200" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="263">
+      <c r="B14" s="258">
         <f>'Data Input'!I10*C14</f>
         <v>0</v>
       </c>
-      <c r="C14" s="258">
+      <c r="C14" s="253">
         <v>0.4</v>
       </c>
       <c r="E14" s="101" t="s">
@@ -12910,14 +12964,14 @@
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="254" t="s">
+      <c r="A15" s="249" t="s">
         <v>185</v>
       </c>
-      <c r="B15" s="263">
+      <c r="B15" s="258">
         <f>'Data Input'!I11*C15</f>
         <v>0</v>
       </c>
-      <c r="C15" s="259">
+      <c r="C15" s="254">
         <f>IF('Data Input'!I11&lt;12500,100%,0%)</f>
         <v>1</v>
       </c>
@@ -12937,10 +12991,10 @@
       <c r="L15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="351" t="s">
+      <c r="M15" s="350" t="s">
         <v>180</v>
       </c>
-      <c r="N15" s="351"/>
+      <c r="N15" s="350"/>
       <c r="O15" s="106"/>
       <c r="P15" s="233" t="s">
         <v>36</v>
@@ -12953,11 +13007,11 @@
       <c r="A16" s="200" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="263">
+      <c r="B16" s="258">
         <f>'Data Input'!I12*C16</f>
         <v>0</v>
       </c>
-      <c r="C16" s="259">
+      <c r="C16" s="254">
         <f>IF('Data Input'!I12&lt;12500,100%,0%)</f>
         <v>1</v>
       </c>
@@ -12993,11 +13047,11 @@
       <c r="A17" s="200" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="263">
+      <c r="B17" s="258">
         <f>'Data Input'!I14*C17</f>
         <v>0</v>
       </c>
-      <c r="C17" s="259">
+      <c r="C17" s="254">
         <v>1</v>
       </c>
       <c r="E17" s="101" t="s">
@@ -13013,14 +13067,14 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="254" t="s">
+      <c r="A18" s="249" t="s">
         <v>187</v>
       </c>
-      <c r="B18" s="263">
+      <c r="B18" s="258">
         <f>'Data Input'!I15*C18</f>
         <v>0</v>
       </c>
-      <c r="C18" s="259">
+      <c r="C18" s="254">
         <v>1</v>
       </c>
       <c r="E18" s="22" t="s">
@@ -13039,11 +13093,11 @@
       <c r="A19" s="202" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="264">
+      <c r="B19" s="259">
         <f ca="1">IF('Data Input'!I17="",0,'Data Input'!I17*(1+(TODAY()+180-'Data Input'!I18)*C19))</f>
         <v>0</v>
       </c>
-      <c r="C19" s="260">
+      <c r="C19" s="255">
         <f>9%/365</f>
         <v>2.4657534246575342E-4</v>
       </c>
@@ -13111,7 +13165,7 @@
       </c>
       <c r="C22" s="123">
         <f>'Data Input'!C21</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="E22" s="104" t="s">
         <v>15</v>
@@ -13183,7 +13237,7 @@
       </c>
       <c r="C25" s="124"/>
       <c r="D25" s="109"/>
-      <c r="E25" s="277"/>
+      <c r="E25" s="272"/>
       <c r="F25" s="105"/>
       <c r="G25" s="109"/>
       <c r="I25" s="227" t="s">
@@ -13202,7 +13256,7 @@
       <c r="B26" s="121"/>
       <c r="C26" s="128"/>
       <c r="D26" s="109"/>
-      <c r="E26" s="277"/>
+      <c r="E26" s="272"/>
       <c r="F26" s="109"/>
       <c r="G26" s="109"/>
       <c r="I26" s="230" t="s">
@@ -13224,7 +13278,7 @@
       </c>
       <c r="C27" s="124"/>
       <c r="D27" s="108"/>
-      <c r="E27" s="277"/>
+      <c r="E27" s="272"/>
       <c r="F27" s="108"/>
       <c r="G27" s="108"/>
       <c r="I27" s="135"/>
@@ -13240,7 +13294,7 @@
       </c>
       <c r="C28" s="125"/>
       <c r="D28" s="108"/>
-      <c r="E28" s="277"/>
+      <c r="E28" s="272"/>
       <c r="F28" s="106"/>
       <c r="G28" s="108"/>
       <c r="I28" s="223" t="s">
@@ -13258,7 +13312,7 @@
         <v>1250</v>
       </c>
       <c r="C29" s="125"/>
-      <c r="E29" s="277"/>
+      <c r="E29" s="272"/>
       <c r="F29" s="106"/>
       <c r="I29" s="225" t="s">
         <v>167</v>
@@ -13278,7 +13332,7 @@
       </c>
       <c r="B30" s="120"/>
       <c r="C30" s="129"/>
-      <c r="E30" s="277"/>
+      <c r="E30" s="272"/>
       <c r="F30" s="106"/>
       <c r="I30" s="227" t="s">
         <v>8</v>
@@ -13301,7 +13355,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="126"/>
-      <c r="E31" s="277"/>
+      <c r="E31" s="272"/>
       <c r="F31" s="106"/>
       <c r="I31" s="227" t="s">
         <v>17</v>
@@ -13323,7 +13377,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="126"/>
-      <c r="E32" s="277"/>
+      <c r="E32" s="272"/>
       <c r="F32" s="106"/>
       <c r="I32" s="227" t="s">
         <v>171</v>
@@ -13340,7 +13394,7 @@
       </c>
       <c r="B33" s="121"/>
       <c r="C33" s="129"/>
-      <c r="E33" s="277"/>
+      <c r="E33" s="272"/>
       <c r="F33" s="106"/>
       <c r="I33" s="230" t="s">
         <v>143</v>
@@ -13361,7 +13415,7 @@
       </c>
       <c r="C34" s="126"/>
       <c r="D34" s="108"/>
-      <c r="E34" s="278"/>
+      <c r="E34" s="273"/>
       <c r="F34" s="106"/>
       <c r="L34"/>
     </row>
@@ -13375,7 +13429,7 @@
       </c>
       <c r="C35" s="126"/>
       <c r="D35" s="108"/>
-      <c r="E35" s="277"/>
+      <c r="E35" s="272"/>
       <c r="F35" s="106"/>
       <c r="L35"/>
     </row>
@@ -13388,28 +13442,28 @@
         <v>0</v>
       </c>
       <c r="C36" s="127"/>
-      <c r="E36" s="277"/>
+      <c r="E36" s="272"/>
       <c r="F36" s="106"/>
       <c r="L36"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N37" s="277"/>
+      <c r="N37" s="272"/>
       <c r="O37" s="106"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N38" s="278"/>
+      <c r="N38" s="273"/>
       <c r="O38" s="106"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N39" s="277"/>
+      <c r="N39" s="272"/>
       <c r="O39" s="106"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N40" s="277"/>
+      <c r="N40" s="272"/>
       <c r="O40" s="106"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N41" s="279"/>
+      <c r="N41" s="274"/>
       <c r="O41" s="106"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1. update excel 2. disable new properteis from view 3. compile a updated js
</commit_message>
<xml_diff>
--- a/IntranetPortal/IntranetPortal/App_Data/underwriter.xlsx
+++ b/IntranetPortal/IntranetPortal/App_Data/underwriter.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Data Input" sheetId="4" r:id="rId1"/>
     <sheet name="Flip Sheets" sheetId="3" r:id="rId2"/>
     <sheet name="Rental Model" sheetId="7" r:id="rId3"/>
-    <sheet name="Tables" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="Tables" sheetId="2" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="200">
   <si>
     <t>Property Address:</t>
   </si>
@@ -857,7 +857,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1166,6 +1166,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1181,7 +1218,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="356">
+  <cellXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1880,10 +1917,6 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1908,22 +1941,10 @@
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1934,10 +1955,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -2066,26 +2083,10 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -2110,14 +2111,6 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
@@ -2152,6 +2145,46 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -2212,35 +2245,35 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
@@ -2650,7 +2683,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,17 +2753,17 @@
       <c r="B3" s="198" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="250"/>
+      <c r="C3" s="246"/>
       <c r="D3" s="191"/>
-      <c r="E3" s="252" t="s">
+      <c r="E3" s="248" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="253"/>
+      <c r="F3" s="310"/>
       <c r="G3" s="194"/>
       <c r="H3" s="198" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="304"/>
+      <c r="I3" s="310"/>
       <c r="J3" s="164"/>
       <c r="K3" s="196" t="s">
         <v>142</v>
@@ -2751,12 +2784,12 @@
       <c r="E4" s="199" t="s">
         <v>145</v>
       </c>
-      <c r="F4" s="246"/>
+      <c r="F4" s="296"/>
       <c r="G4" s="194"/>
       <c r="H4" s="200" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="305"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="164"/>
       <c r="K4" s="164"/>
       <c r="L4" s="165"/>
@@ -2772,17 +2805,19 @@
       <c r="E5" s="200" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="240"/>
+      <c r="F5" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G5" s="194"/>
       <c r="H5" s="200" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="305"/>
+      <c r="I5" s="312"/>
       <c r="J5" s="164"/>
-      <c r="K5" s="318" t="s">
+      <c r="K5" s="317" t="s">
         <v>173</v>
       </c>
-      <c r="L5" s="319"/>
+      <c r="L5" s="318"/>
       <c r="M5" s="164"/>
       <c r="O5" s="221"/>
     </row>
@@ -2791,22 +2826,24 @@
       <c r="B6" s="201" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="251"/>
+      <c r="C6" s="247"/>
       <c r="D6" s="191"/>
       <c r="E6" s="200" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="240"/>
+      <c r="F6" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G6" s="194"/>
       <c r="H6" s="200" t="s">
         <v>196</v>
       </c>
-      <c r="I6" s="305"/>
+      <c r="I6" s="312"/>
       <c r="J6" s="164"/>
-      <c r="K6" s="265" t="s">
+      <c r="K6" s="260" t="s">
         <v>167</v>
       </c>
-      <c r="L6" s="266" t="e">
+      <c r="L6" s="261" t="e">
         <f ca="1">SUM(Tables!B6:B25)</f>
         <v>#VALUE!</v>
       </c>
@@ -2822,17 +2859,19 @@
       <c r="E7" s="200" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="306"/>
+      <c r="F7" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G7" s="194"/>
       <c r="H7" s="200" t="s">
         <v>190</v>
       </c>
-      <c r="I7" s="305"/>
+      <c r="I7" s="312"/>
       <c r="J7" s="164"/>
-      <c r="K7" s="267" t="s">
+      <c r="K7" s="262" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="268" t="e">
+      <c r="L7" s="263" t="e">
         <f ca="1">'Flip Sheets'!C26</f>
         <v>#VALUE!</v>
       </c>
@@ -2845,20 +2884,22 @@
       </c>
       <c r="C8" s="238"/>
       <c r="D8" s="191"/>
-      <c r="E8" s="255" t="s">
+      <c r="E8" s="250" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="293"/>
+      <c r="F8" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G8" s="194"/>
       <c r="H8" s="200" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="305"/>
+      <c r="I8" s="312"/>
       <c r="J8" s="164"/>
-      <c r="K8" s="267" t="s">
+      <c r="K8" s="262" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="268" t="e">
+      <c r="L8" s="263" t="e">
         <f ca="1">'Flip Sheets'!H23</f>
         <v>#VALUE!</v>
       </c>
@@ -2866,25 +2907,27 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="188"/>
-      <c r="B9" s="255" t="s">
+      <c r="B9" s="250" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="293"/>
+      <c r="C9" s="288"/>
       <c r="D9" s="191"/>
       <c r="E9" s="200" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="240"/>
+      <c r="F9" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G9" s="194"/>
       <c r="H9" s="200" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="305"/>
+      <c r="I9" s="312"/>
       <c r="J9" s="164"/>
-      <c r="K9" s="267" t="s">
+      <c r="K9" s="262" t="s">
         <v>171</v>
       </c>
-      <c r="L9" s="269" t="e">
+      <c r="L9" s="264" t="e">
         <f ca="1">'Flip Sheets'!F26</f>
         <v>#VALUE!</v>
       </c>
@@ -2892,25 +2935,27 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="188"/>
-      <c r="B10" s="255" t="s">
+      <c r="B10" s="250" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="293"/>
+      <c r="C10" s="288"/>
       <c r="D10" s="191"/>
       <c r="E10" s="200" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="240"/>
+      <c r="F10" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G10" s="194"/>
       <c r="H10" s="200" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="305"/>
+      <c r="I10" s="312"/>
       <c r="J10" s="164"/>
-      <c r="K10" s="270" t="s">
+      <c r="K10" s="265" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="271" t="e">
+      <c r="L10" s="266" t="e">
         <f ca="1">'Flip Sheets'!H25</f>
         <v>#VALUE!</v>
       </c>
@@ -2921,17 +2966,19 @@
       <c r="B11" s="200" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="294"/>
+      <c r="C11" s="289"/>
       <c r="D11" s="191"/>
       <c r="E11" s="200" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="240"/>
+      <c r="F11" s="239" t="s">
+        <v>67</v>
+      </c>
       <c r="G11" s="194"/>
-      <c r="H11" s="254" t="s">
+      <c r="H11" s="249" t="s">
         <v>185</v>
       </c>
-      <c r="I11" s="305"/>
+      <c r="I11" s="312"/>
       <c r="J11" s="164"/>
       <c r="K11" s="157"/>
       <c r="L11" s="158"/>
@@ -2942,22 +2989,22 @@
       <c r="B12" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="303"/>
+      <c r="C12" s="294"/>
       <c r="D12" s="191"/>
       <c r="E12" s="200" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="240"/>
+      <c r="F12" s="239"/>
       <c r="G12" s="194"/>
       <c r="H12" s="200" t="s">
         <v>189</v>
       </c>
-      <c r="I12" s="305"/>
+      <c r="I12" s="296"/>
       <c r="J12" s="164"/>
-      <c r="K12" s="320" t="s">
+      <c r="K12" s="319" t="s">
         <v>172</v>
       </c>
-      <c r="L12" s="321"/>
+      <c r="L12" s="320"/>
       <c r="M12" s="164"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2965,7 +3012,7 @@
       <c r="B13" s="200" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="240"/>
+      <c r="C13" s="239"/>
       <c r="D13" s="191"/>
       <c r="E13" s="201" t="s">
         <v>147</v>
@@ -2975,7 +3022,9 @@
       <c r="H13" s="200" t="s">
         <v>186</v>
       </c>
-      <c r="I13" s="240"/>
+      <c r="I13" s="315" t="s">
+        <v>67</v>
+      </c>
       <c r="J13" s="164"/>
       <c r="K13" s="203" t="s">
         <v>167</v>
@@ -2991,19 +3040,19 @@
       <c r="B14" s="199" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="240" t="s">
+      <c r="C14" s="239" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="207"/>
       <c r="E14" s="200" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="247"/>
+      <c r="F14" s="245"/>
       <c r="G14" s="194"/>
       <c r="H14" s="200" t="s">
         <v>188</v>
       </c>
-      <c r="I14" s="305"/>
+      <c r="I14" s="312"/>
       <c r="J14" s="164"/>
       <c r="K14" s="159" t="s">
         <v>8</v>
@@ -3019,17 +3068,17 @@
       <c r="B15" s="202" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="241"/>
+      <c r="C15" s="240"/>
       <c r="D15" s="207"/>
       <c r="E15" s="200" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="247"/>
+      <c r="F15" s="245"/>
       <c r="G15" s="194"/>
-      <c r="H15" s="254" t="s">
+      <c r="H15" s="249" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="306"/>
+      <c r="I15" s="296"/>
       <c r="J15" s="164"/>
       <c r="K15" s="159" t="s">
         <v>17</v>
@@ -3048,12 +3097,14 @@
       <c r="E16" s="209" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="306"/>
+      <c r="F16" s="307"/>
       <c r="G16" s="194"/>
       <c r="H16" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="I16" s="240"/>
+      <c r="I16" s="315" t="s">
+        <v>67</v>
+      </c>
       <c r="J16" s="164"/>
       <c r="K16" s="159" t="s">
         <v>171</v>
@@ -3074,12 +3125,12 @@
       <c r="E17" s="200" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="248"/>
+      <c r="F17" s="309"/>
       <c r="G17" s="194"/>
       <c r="H17" s="200" t="s">
         <v>102</v>
       </c>
-      <c r="I17" s="305"/>
+      <c r="I17" s="312"/>
       <c r="J17" s="164"/>
       <c r="K17" s="160" t="s">
         <v>143</v>
@@ -3100,12 +3151,12 @@
       <c r="E18" s="200" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="239"/>
+      <c r="F18" s="296"/>
       <c r="G18" s="164"/>
       <c r="H18" s="208" t="s">
         <v>135</v>
       </c>
-      <c r="I18" s="307"/>
+      <c r="I18" s="316"/>
       <c r="J18" s="164"/>
       <c r="K18" s="212"/>
       <c r="L18" s="165"/>
@@ -3113,24 +3164,23 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="188"/>
-      <c r="B19" s="255" t="s">
+      <c r="B19" s="250" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="293" t="str">
-        <f>IF(OR('Data Input'!C14="Yes",'Data Input'!C15&gt;0)*AND('Data Input'!F9&lt;&gt;"Yes",'Data Input'!F10&lt;&gt;"Yes",'Data Input'!F11&lt;&gt;"Yes",'Data Input'!C20&lt;&gt;"",'Data Input'!C20&gt;0),"Yes","No")</f>
-        <v>No</v>
+      <c r="C19" s="311" t="s">
+        <v>67</v>
       </c>
       <c r="D19" s="191"/>
       <c r="E19" s="200" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="248"/>
+      <c r="F19" s="309"/>
       <c r="G19" s="188"/>
       <c r="J19" s="164"/>
-      <c r="K19" s="322" t="s">
+      <c r="K19" s="321" t="s">
         <v>194</v>
       </c>
-      <c r="L19" s="323"/>
+      <c r="L19" s="322"/>
       <c r="M19" s="164"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3143,15 +3193,15 @@
       <c r="E20" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="249"/>
+      <c r="F20" s="313"/>
       <c r="G20" s="188"/>
       <c r="H20" s="164"/>
       <c r="I20" s="164"/>
       <c r="J20" s="164"/>
-      <c r="K20" s="272" t="s">
+      <c r="K20" s="267" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="291" t="e">
+      <c r="L20" s="286" t="e">
         <f ca="1">'Flip Sheets'!C33</f>
         <v>#VALUE!</v>
       </c>
@@ -3159,18 +3209,18 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="188"/>
-      <c r="B21" s="255" t="s">
+      <c r="B21" s="250" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="297">
-        <v>0.75</v>
+      <c r="C21" s="290">
+        <v>0</v>
       </c>
       <c r="D21" s="194"/>
       <c r="J21" s="164"/>
-      <c r="K21" s="274" t="s">
+      <c r="K21" s="269" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="273" t="e">
+      <c r="L21" s="268" t="e">
         <f ca="1">'Flip Sheets'!F33</f>
         <v>#VALUE!</v>
       </c>
@@ -3181,7 +3231,7 @@
       <c r="B22" s="209" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="298"/>
+      <c r="C22" s="312"/>
       <c r="D22" s="194"/>
       <c r="E22" s="215" t="s">
         <v>61</v>
@@ -3191,10 +3241,10 @@
       <c r="H22" s="217"/>
       <c r="I22" s="218"/>
       <c r="J22" s="164"/>
-      <c r="K22" s="275" t="s">
+      <c r="K22" s="270" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="292" t="e">
+      <c r="L22" s="287" t="e">
         <f ca="1">'Flip Sheets'!H33</f>
         <v>#VALUE!</v>
       </c>
@@ -3205,16 +3255,16 @@
       <c r="B23" s="211" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="249"/>
+      <c r="C23" s="313"/>
       <c r="D23" s="194"/>
-      <c r="E23" s="324"/>
-      <c r="F23" s="325"/>
-      <c r="G23" s="325"/>
-      <c r="H23" s="325"/>
-      <c r="I23" s="326"/>
+      <c r="E23" s="323"/>
+      <c r="F23" s="324"/>
+      <c r="G23" s="324"/>
+      <c r="H23" s="324"/>
+      <c r="I23" s="325"/>
       <c r="J23" s="164"/>
-      <c r="K23" s="289"/>
-      <c r="L23" s="290"/>
+      <c r="K23" s="284"/>
+      <c r="L23" s="285"/>
       <c r="M23" s="164"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3222,16 +3272,16 @@
       <c r="B24" s="164"/>
       <c r="C24" s="213"/>
       <c r="D24" s="194"/>
-      <c r="E24" s="327"/>
-      <c r="F24" s="328"/>
-      <c r="G24" s="328"/>
-      <c r="H24" s="328"/>
-      <c r="I24" s="329"/>
+      <c r="E24" s="326"/>
+      <c r="F24" s="327"/>
+      <c r="G24" s="327"/>
+      <c r="H24" s="327"/>
+      <c r="I24" s="328"/>
       <c r="J24" s="164"/>
-      <c r="K24" s="316" t="s">
+      <c r="K24" s="305" t="s">
         <v>178</v>
       </c>
-      <c r="L24" s="317" t="e">
+      <c r="L24" s="306" t="e">
         <f ca="1">Tables!J22-Tables!J29</f>
         <v>#VALUE!</v>
       </c>
@@ -3244,11 +3294,11 @@
       </c>
       <c r="C25" s="214"/>
       <c r="D25" s="194"/>
-      <c r="E25" s="327"/>
-      <c r="F25" s="328"/>
-      <c r="G25" s="328"/>
-      <c r="H25" s="328"/>
-      <c r="I25" s="329"/>
+      <c r="E25" s="326"/>
+      <c r="F25" s="327"/>
+      <c r="G25" s="327"/>
+      <c r="H25" s="327"/>
+      <c r="I25" s="328"/>
       <c r="J25" s="164"/>
       <c r="K25" s="164"/>
       <c r="L25" s="165"/>
@@ -3256,31 +3306,31 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="188"/>
-      <c r="B26" s="276" t="s">
+      <c r="B26" s="271" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="299"/>
+      <c r="C26" s="295"/>
       <c r="D26" s="194"/>
-      <c r="E26" s="327"/>
-      <c r="F26" s="328"/>
-      <c r="G26" s="328"/>
-      <c r="H26" s="328"/>
-      <c r="I26" s="329"/>
+      <c r="E26" s="326"/>
+      <c r="F26" s="327"/>
+      <c r="G26" s="327"/>
+      <c r="H26" s="327"/>
+      <c r="I26" s="328"/>
       <c r="J26" s="164"/>
       <c r="M26" s="164"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="188"/>
-      <c r="B27" s="200" t="s">
+      <c r="B27" s="308" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="296"/>
+      <c r="C27" s="314"/>
       <c r="D27" s="194"/>
-      <c r="E27" s="327"/>
-      <c r="F27" s="328"/>
-      <c r="G27" s="328"/>
-      <c r="H27" s="328"/>
-      <c r="I27" s="329"/>
+      <c r="E27" s="326"/>
+      <c r="F27" s="327"/>
+      <c r="G27" s="327"/>
+      <c r="H27" s="327"/>
+      <c r="I27" s="328"/>
       <c r="J27" s="164"/>
       <c r="K27" s="219"/>
       <c r="L27" s="220"/>
@@ -3293,27 +3343,29 @@
       </c>
       <c r="C28" s="296"/>
       <c r="D28" s="194"/>
-      <c r="E28" s="327"/>
-      <c r="F28" s="328"/>
-      <c r="G28" s="328"/>
-      <c r="H28" s="328"/>
-      <c r="I28" s="329"/>
+      <c r="E28" s="326"/>
+      <c r="F28" s="327"/>
+      <c r="G28" s="327"/>
+      <c r="H28" s="327"/>
+      <c r="I28" s="328"/>
       <c r="J28" s="164"/>
       <c r="K28" s="219"/>
       <c r="M28" s="164"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="188"/>
-      <c r="B29" s="255" t="s">
+      <c r="B29" s="250" t="s">
         <v>195</v>
       </c>
-      <c r="C29" s="240"/>
+      <c r="C29" s="237" t="s">
+        <v>67</v>
+      </c>
       <c r="D29" s="194"/>
-      <c r="E29" s="327"/>
-      <c r="F29" s="328"/>
-      <c r="G29" s="328"/>
-      <c r="H29" s="328"/>
-      <c r="I29" s="329"/>
+      <c r="E29" s="326"/>
+      <c r="F29" s="327"/>
+      <c r="G29" s="327"/>
+      <c r="H29" s="327"/>
+      <c r="I29" s="328"/>
       <c r="J29" s="164"/>
       <c r="K29" s="219"/>
       <c r="L29" s="222"/>
@@ -3324,15 +3376,13 @@
       <c r="B30" s="200" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="300">
-        <v>6</v>
-      </c>
+      <c r="C30" s="291"/>
       <c r="D30" s="194"/>
-      <c r="E30" s="327"/>
-      <c r="F30" s="328"/>
-      <c r="G30" s="328"/>
-      <c r="H30" s="328"/>
-      <c r="I30" s="329"/>
+      <c r="E30" s="326"/>
+      <c r="F30" s="327"/>
+      <c r="G30" s="327"/>
+      <c r="H30" s="327"/>
+      <c r="I30" s="328"/>
       <c r="J30" s="164"/>
       <c r="K30" s="219"/>
       <c r="L30" s="220"/>
@@ -3343,15 +3393,15 @@
       <c r="B31" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="301">
+      <c r="C31" s="292">
         <v>0.05</v>
       </c>
       <c r="D31" s="194"/>
-      <c r="E31" s="327"/>
-      <c r="F31" s="328"/>
-      <c r="G31" s="328"/>
-      <c r="H31" s="328"/>
-      <c r="I31" s="329"/>
+      <c r="E31" s="326"/>
+      <c r="F31" s="327"/>
+      <c r="G31" s="327"/>
+      <c r="H31" s="327"/>
+      <c r="I31" s="328"/>
       <c r="J31" s="164"/>
       <c r="K31" s="219"/>
       <c r="L31" s="220"/>
@@ -3362,15 +3412,15 @@
       <c r="B32" s="208" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="302">
+      <c r="C32" s="293">
         <v>0.35</v>
       </c>
       <c r="D32" s="194"/>
-      <c r="E32" s="330"/>
-      <c r="F32" s="331"/>
-      <c r="G32" s="331"/>
-      <c r="H32" s="331"/>
-      <c r="I32" s="332"/>
+      <c r="E32" s="329"/>
+      <c r="F32" s="330"/>
+      <c r="G32" s="330"/>
+      <c r="H32" s="330"/>
+      <c r="I32" s="331"/>
       <c r="J32" s="164"/>
       <c r="K32" s="219"/>
       <c r="L32" s="220"/>
@@ -3387,7 +3437,7 @@
       <c r="M34" s="147"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="plRIxWnjwlPp/Gyc+sZf1BpkoQrRT8zKRaBxPrgANaelZPQYIe+JOeyFqmLYBHpYVxPB2VEv31DyQqIH6h63Mg==" saltValue="QXZ8wZvYmKXkCUN0nfdsbA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <dataConsolidate/>
   <mergeCells count="4">
     <mergeCell ref="K5:L5"/>
@@ -3400,7 +3450,7 @@
     <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F20 F18 C27:C28 I14 C12 C23 I17 C20 C18 C30 I3:I12">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18 I17 C22:C23 I3:I12 C12 C20 I14:I15 C18 F3:F4 C30 F20 C26:C28">
       <formula1>-1000000</formula1>
     </dataValidation>
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C15">
@@ -3418,48 +3468,42 @@
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$8</xm:f>
           </x14:formula1>
           <xm:sqref>C13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F6</xm:sqref>
+          <xm:sqref>C29 F5:F11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Tables!$J$2:$J$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
           <xm:sqref>I16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
           <xm:sqref>C14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
           <xm:sqref>I13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Tables!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F9:F11</xm:sqref>
+          <xm:sqref>C19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3472,7 +3516,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I41"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3505,13 +3549,13 @@
       <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="335">
+      <c r="C2" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D2" s="335"/>
-      <c r="E2" s="335"/>
-      <c r="F2" s="336"/>
+      <c r="D2" s="332"/>
+      <c r="E2" s="332"/>
+      <c r="F2" s="333"/>
       <c r="G2" s="43"/>
       <c r="H2" s="44" t="s">
         <v>44</v>
@@ -3523,8 +3567,8 @@
       <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="311">
-        <f>'Data Input'!C4</f>
+      <c r="C3" s="300">
+        <f>'Data Input'!C5</f>
         <v>0</v>
       </c>
       <c r="D3" s="25"/>
@@ -3537,22 +3581,22 @@
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="84">
-        <f>'Data Input'!C28</f>
+        <f>'Data Input'!C30</f>
         <v>0</v>
       </c>
       <c r="I3" s="39"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39"/>
-      <c r="B4" s="339" t="s">
+      <c r="B4" s="336" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="340"/>
+      <c r="C4" s="337"/>
       <c r="D4" s="48"/>
-      <c r="E4" s="339" t="s">
+      <c r="E4" s="336" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="340"/>
+      <c r="F4" s="337"/>
       <c r="G4" s="49"/>
       <c r="H4" s="50" t="s">
         <v>42</v>
@@ -3745,13 +3789,13 @@
       <c r="B15" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="335">
+      <c r="C15" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D15" s="335"/>
-      <c r="E15" s="335"/>
-      <c r="F15" s="336"/>
+      <c r="D15" s="332"/>
+      <c r="E15" s="332"/>
+      <c r="F15" s="333"/>
       <c r="G15" s="43"/>
       <c r="H15" s="138" t="s">
         <v>44</v>
@@ -3763,7 +3807,7 @@
       <c r="B16" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="311">
+      <c r="C16" s="300">
         <f>'Data Input'!C4</f>
         <v>0</v>
       </c>
@@ -3777,22 +3821,22 @@
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="139">
-        <f>'Data Input'!C28</f>
+        <f>'Data Input'!C30</f>
         <v>0</v>
       </c>
       <c r="I16" s="39"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39"/>
-      <c r="B17" s="337" t="s">
+      <c r="B17" s="334" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="338"/>
+      <c r="C17" s="335"/>
       <c r="D17" s="48"/>
-      <c r="E17" s="337" t="s">
+      <c r="E17" s="334" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="338"/>
+      <c r="F17" s="335"/>
       <c r="G17" s="59"/>
       <c r="H17" s="60" t="s">
         <v>62</v>
@@ -4026,13 +4070,13 @@
       <c r="B30" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="335">
+      <c r="C30" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D30" s="335"/>
-      <c r="E30" s="335"/>
-      <c r="F30" s="336"/>
+      <c r="D30" s="332"/>
+      <c r="E30" s="332"/>
+      <c r="F30" s="333"/>
       <c r="G30" s="43"/>
       <c r="H30" s="64"/>
       <c r="I30" s="39"/>
@@ -4042,7 +4086,7 @@
       <c r="B31" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="311">
+      <c r="C31" s="300">
         <f>'Data Input'!C4</f>
         <v>0</v>
       </c>
@@ -4060,15 +4104,15 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39"/>
-      <c r="B32" s="333" t="s">
+      <c r="B32" s="338" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="334"/>
+      <c r="C32" s="339"/>
       <c r="D32" s="48"/>
-      <c r="E32" s="333" t="s">
+      <c r="E32" s="338" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="334"/>
+      <c r="F32" s="339"/>
       <c r="G32" s="49"/>
       <c r="H32" s="67" t="s">
         <v>40</v>
@@ -4112,15 +4156,15 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="39"/>
-      <c r="B35" s="333" t="s">
+      <c r="B35" s="338" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="334"/>
+      <c r="C35" s="339"/>
       <c r="D35" s="48"/>
-      <c r="E35" s="333" t="s">
+      <c r="E35" s="338" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="334"/>
+      <c r="F35" s="339"/>
       <c r="G35" s="49"/>
       <c r="H35" s="67" t="s">
         <v>54</v>
@@ -4254,19 +4298,19 @@
       <c r="I41" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6AkjZXVSFB0ziVOXcrpeHhh/HLATkbQVxrQZuEWcVLXwzsunA6rRgTpZldJaFHDBfmDujtzSf7DiifC4AGzaPQ==" saltValue="N+SbVL6VG7pgvFTwtEdyCA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="11">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="E38:E39">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
@@ -4284,7 +4328,7 @@
   <dimension ref="A1:O399"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4326,14 +4370,14 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="312" t="s">
+      <c r="B2" s="301" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="313"/>
-      <c r="E2" s="341" t="s">
+      <c r="C2" s="302"/>
+      <c r="E2" s="340" t="s">
         <v>197</v>
       </c>
-      <c r="F2" s="342"/>
+      <c r="F2" s="341"/>
       <c r="J2" s="163"/>
       <c r="K2" s="164">
         <v>1</v>
@@ -4351,14 +4395,16 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="314" t="s">
+      <c r="B3" s="303" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="242"/>
-      <c r="E3" s="281" t="s">
+      <c r="C3" s="241">
+        <v>0</v>
+      </c>
+      <c r="E3" s="276" t="s">
         <v>198</v>
       </c>
-      <c r="F3" s="287">
+      <c r="F3" s="282">
         <f>C18</f>
         <v>0</v>
       </c>
@@ -4384,16 +4430,16 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="255" t="s">
+      <c r="B4" s="250" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="243" t="s">
+      <c r="C4" s="242" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="283" t="s">
+      <c r="E4" s="278" t="s">
         <v>199</v>
       </c>
-      <c r="F4" s="282">
+      <c r="F4" s="277">
         <f>F20</f>
         <v>-110</v>
       </c>
@@ -4419,14 +4465,16 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="314" t="s">
+      <c r="B5" s="303" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="242"/>
-      <c r="E5" s="283" t="s">
+      <c r="C5" s="241">
+        <v>0</v>
+      </c>
+      <c r="E5" s="278" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="286" t="e">
+      <c r="F5" s="281" t="e">
         <f>H12</f>
         <v>#N/A</v>
       </c>
@@ -4452,16 +4500,18 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="314" t="s">
+      <c r="B6" s="303" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="244"/>
-      <c r="E6" s="283" t="s">
+      <c r="C6" s="243">
+        <v>0</v>
+      </c>
+      <c r="E6" s="278" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="284" t="e">
+      <c r="F6" s="279">
         <f>H14</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="J6" s="163"/>
       <c r="K6" s="164">
@@ -4485,14 +4535,16 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="314" t="s">
+      <c r="B7" s="303" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="242"/>
-      <c r="E7" s="285" t="s">
+      <c r="C7" s="241">
+        <v>0</v>
+      </c>
+      <c r="E7" s="280" t="s">
         <v>170</v>
       </c>
-      <c r="F7" s="288" t="e">
+      <c r="F7" s="283" t="e">
         <f>H16</f>
         <v>#N/A</v>
       </c>
@@ -4518,10 +4570,12 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="315" t="s">
+      <c r="B8" s="304" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="245"/>
+      <c r="C8" s="244">
+        <v>0</v>
+      </c>
       <c r="J8" s="163"/>
       <c r="K8" s="164">
         <v>7</v>
@@ -4601,13 +4655,13 @@
       <c r="B11" s="167" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="335">
+      <c r="C11" s="332">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D11" s="335"/>
-      <c r="E11" s="335"/>
-      <c r="F11" s="336"/>
+      <c r="D11" s="332"/>
+      <c r="E11" s="332"/>
+      <c r="F11" s="333"/>
       <c r="G11" s="39"/>
       <c r="H11" s="148" t="s">
         <v>165</v>
@@ -4639,11 +4693,11 @@
       <c r="B12" s="168" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="347">
+      <c r="C12" s="346">
         <f>'Rental Model'!C6</f>
         <v>0</v>
       </c>
-      <c r="D12" s="347"/>
+      <c r="D12" s="346"/>
       <c r="E12" s="41" t="s">
         <v>158</v>
       </c>
@@ -4682,11 +4736,11 @@
       <c r="B13" s="170" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="348" t="e">
+      <c r="C13" s="347">
         <f>IF('Rental Model'!C8="",MATCH(1,INDEX(--(O2:O97&gt;F13),0),0),'Rental Model'!C7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D13" s="348"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="347"/>
       <c r="E13" s="171" t="s">
         <v>169</v>
       </c>
@@ -4720,19 +4774,19 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="39"/>
-      <c r="B14" s="343" t="s">
+      <c r="B14" s="342" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="344"/>
+      <c r="C14" s="343"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="345" t="s">
+      <c r="E14" s="344" t="s">
         <v>160</v>
       </c>
-      <c r="F14" s="346"/>
+      <c r="F14" s="345"/>
       <c r="G14" s="39"/>
-      <c r="H14" s="150" t="e">
+      <c r="H14" s="150">
         <f>C13</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="I14" s="39"/>
       <c r="K14" s="164">
@@ -4760,7 +4814,7 @@
       <c r="B15" s="173" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="280">
+      <c r="C15" s="275">
         <f>'Rental Model'!C3</f>
         <v>0</v>
       </c>
@@ -4768,7 +4822,7 @@
       <c r="E15" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="F15" s="280">
+      <c r="F15" s="275">
         <f>'Rental Model'!C7</f>
         <v>0</v>
       </c>
@@ -4802,7 +4856,7 @@
       <c r="B16" s="176" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="280">
+      <c r="C16" s="275">
         <f>'Rental Model'!C5</f>
         <v>0</v>
       </c>
@@ -4886,7 +4940,7 @@
       <c r="B18" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="280">
+      <c r="C18" s="275">
         <f>SUM(C15:C17)</f>
         <v>0</v>
       </c>
@@ -12368,13 +12422,13 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
@@ -12398,19 +12452,19 @@
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="349">
+      <c r="B1" s="348">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="C1" s="350"/>
-      <c r="D1" s="350"/>
-      <c r="E1" s="350"/>
+      <c r="C1" s="349"/>
+      <c r="D1" s="349"/>
+      <c r="E1" s="349"/>
       <c r="F1" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="308">
+      <c r="G1" s="297">
         <f>'Data Input'!C30</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I1" s="90" t="s">
         <v>108</v>
@@ -12418,10 +12472,10 @@
       <c r="J1" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="352" t="s">
+      <c r="L1" s="351" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="353"/>
+      <c r="M1" s="352"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -12444,7 +12498,7 @@
       <c r="F2" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="309">
+      <c r="G2" s="298">
         <f>'Data Input'!C32</f>
         <v>0.35</v>
       </c>
@@ -12453,14 +12507,14 @@
       <c r="L2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="351" t="s">
+      <c r="M2" s="350" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="351"/>
-      <c r="O2" s="354" t="s">
+      <c r="N2" s="350"/>
+      <c r="O2" s="353" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="354"/>
+      <c r="P2" s="353"/>
       <c r="Q2" s="8"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12482,7 +12536,7 @@
       <c r="F3" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="310">
+      <c r="G3" s="299">
         <v>0</v>
       </c>
       <c r="I3" s="92" t="s">
@@ -12495,16 +12549,16 @@
         <f ca="1">Tables!B6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M3" s="355" t="e">
+      <c r="M3" s="354" t="e">
         <f ca="1">IF(Tables!F13&gt;=Tables!B6,Tables!B6,Tables!F13)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N3" s="355"/>
-      <c r="O3" s="355" t="e">
+      <c r="N3" s="354"/>
+      <c r="O3" s="354" t="e">
         <f ca="1">Tables!F13-Tables!M3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P3" s="355"/>
+      <c r="P3" s="354"/>
       <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12556,14 +12610,14 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="261" t="s">
+      <c r="A6" s="256" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="262" t="e">
+      <c r="B6" s="257" t="e">
         <f ca="1">(F6-SUM(B7:B19,B21:B25,B28:B29,B31:B32,B34:B36,F7:F11)-(SUM(B7:B19,B21:B25,B28:B29,B31:B32,B34:B36)*G2))/((G2*1.0058)+1.0058)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C6" s="256">
+      <c r="C6" s="251">
         <v>1</v>
       </c>
       <c r="E6" s="101" t="s">
@@ -12601,11 +12655,11 @@
       <c r="A7" s="200" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="263">
+      <c r="B7" s="258">
         <f>'Data Input'!I3*(1+(C7*'Data Input'!C30))</f>
         <v>0</v>
       </c>
-      <c r="C7" s="257">
+      <c r="C7" s="252">
         <f>0.09/12</f>
         <v>7.4999999999999997E-3</v>
       </c>
@@ -12643,11 +12697,11 @@
       <c r="A8" s="200" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="263">
+      <c r="B8" s="258">
         <f>'Data Input'!I4*C8</f>
         <v>0</v>
       </c>
-      <c r="C8" s="258">
+      <c r="C8" s="253">
         <v>1</v>
       </c>
       <c r="E8" s="101" t="s">
@@ -12685,11 +12739,11 @@
       <c r="A9" s="200" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="263">
+      <c r="B9" s="258">
         <f>'Data Input'!I5*C9</f>
         <v>0</v>
       </c>
-      <c r="C9" s="258">
+      <c r="C9" s="253">
         <v>1</v>
       </c>
       <c r="E9" s="101" t="s">
@@ -12725,11 +12779,11 @@
       <c r="A10" s="200" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="263">
+      <c r="B10" s="258">
         <f>'Data Input'!I6*C10</f>
         <v>0</v>
       </c>
-      <c r="C10" s="258">
+      <c r="C10" s="253">
         <v>1</v>
       </c>
       <c r="E10" s="101" t="s">
@@ -12767,11 +12821,11 @@
       <c r="A11" s="200" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="263">
+      <c r="B11" s="258">
         <f>'Data Input'!I7*C11</f>
         <v>0</v>
       </c>
-      <c r="C11" s="258">
+      <c r="C11" s="253">
         <v>1</v>
       </c>
       <c r="E11" s="101" t="s">
@@ -12812,11 +12866,11 @@
       <c r="A12" s="200" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="263">
+      <c r="B12" s="258">
         <f>'Data Input'!I8*C12</f>
         <v>0</v>
       </c>
-      <c r="C12" s="258">
+      <c r="C12" s="253">
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -12848,11 +12902,11 @@
       <c r="A13" s="200" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="263">
+      <c r="B13" s="258">
         <f>'Data Input'!I9*C13</f>
         <v>0</v>
       </c>
-      <c r="C13" s="258">
+      <c r="C13" s="253">
         <v>0.15</v>
       </c>
       <c r="E13" s="101" t="s">
@@ -12883,11 +12937,11 @@
       <c r="A14" s="200" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="263">
+      <c r="B14" s="258">
         <f>'Data Input'!I10*C14</f>
         <v>0</v>
       </c>
-      <c r="C14" s="258">
+      <c r="C14" s="253">
         <v>0.4</v>
       </c>
       <c r="E14" s="101" t="s">
@@ -12910,14 +12964,14 @@
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="254" t="s">
+      <c r="A15" s="249" t="s">
         <v>185</v>
       </c>
-      <c r="B15" s="263">
+      <c r="B15" s="258">
         <f>'Data Input'!I11*C15</f>
         <v>0</v>
       </c>
-      <c r="C15" s="259">
+      <c r="C15" s="254">
         <f>IF('Data Input'!I11&lt;12500,100%,0%)</f>
         <v>1</v>
       </c>
@@ -12937,10 +12991,10 @@
       <c r="L15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="351" t="s">
+      <c r="M15" s="350" t="s">
         <v>180</v>
       </c>
-      <c r="N15" s="351"/>
+      <c r="N15" s="350"/>
       <c r="O15" s="106"/>
       <c r="P15" s="233" t="s">
         <v>36</v>
@@ -12953,11 +13007,11 @@
       <c r="A16" s="200" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="263">
+      <c r="B16" s="258">
         <f>'Data Input'!I12*C16</f>
         <v>0</v>
       </c>
-      <c r="C16" s="259">
+      <c r="C16" s="254">
         <f>IF('Data Input'!I12&lt;12500,100%,0%)</f>
         <v>1</v>
       </c>
@@ -12993,11 +13047,11 @@
       <c r="A17" s="200" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="263">
+      <c r="B17" s="258">
         <f>'Data Input'!I14*C17</f>
         <v>0</v>
       </c>
-      <c r="C17" s="259">
+      <c r="C17" s="254">
         <v>1</v>
       </c>
       <c r="E17" s="101" t="s">
@@ -13013,14 +13067,14 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="254" t="s">
+      <c r="A18" s="249" t="s">
         <v>187</v>
       </c>
-      <c r="B18" s="263">
+      <c r="B18" s="258">
         <f>'Data Input'!I15*C18</f>
         <v>0</v>
       </c>
-      <c r="C18" s="259">
+      <c r="C18" s="254">
         <v>1</v>
       </c>
       <c r="E18" s="22" t="s">
@@ -13039,11 +13093,11 @@
       <c r="A19" s="202" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="264">
+      <c r="B19" s="259">
         <f ca="1">IF('Data Input'!I17="",0,'Data Input'!I17*(1+(TODAY()+180-'Data Input'!I18)*C19))</f>
         <v>0</v>
       </c>
-      <c r="C19" s="260">
+      <c r="C19" s="255">
         <f>9%/365</f>
         <v>2.4657534246575342E-4</v>
       </c>
@@ -13111,7 +13165,7 @@
       </c>
       <c r="C22" s="123">
         <f>'Data Input'!C21</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="E22" s="104" t="s">
         <v>15</v>
@@ -13183,7 +13237,7 @@
       </c>
       <c r="C25" s="124"/>
       <c r="D25" s="109"/>
-      <c r="E25" s="277"/>
+      <c r="E25" s="272"/>
       <c r="F25" s="105"/>
       <c r="G25" s="109"/>
       <c r="I25" s="227" t="s">
@@ -13202,7 +13256,7 @@
       <c r="B26" s="121"/>
       <c r="C26" s="128"/>
       <c r="D26" s="109"/>
-      <c r="E26" s="277"/>
+      <c r="E26" s="272"/>
       <c r="F26" s="109"/>
       <c r="G26" s="109"/>
       <c r="I26" s="230" t="s">
@@ -13224,7 +13278,7 @@
       </c>
       <c r="C27" s="124"/>
       <c r="D27" s="108"/>
-      <c r="E27" s="277"/>
+      <c r="E27" s="272"/>
       <c r="F27" s="108"/>
       <c r="G27" s="108"/>
       <c r="I27" s="135"/>
@@ -13240,7 +13294,7 @@
       </c>
       <c r="C28" s="125"/>
       <c r="D28" s="108"/>
-      <c r="E28" s="277"/>
+      <c r="E28" s="272"/>
       <c r="F28" s="106"/>
       <c r="G28" s="108"/>
       <c r="I28" s="223" t="s">
@@ -13258,7 +13312,7 @@
         <v>1250</v>
       </c>
       <c r="C29" s="125"/>
-      <c r="E29" s="277"/>
+      <c r="E29" s="272"/>
       <c r="F29" s="106"/>
       <c r="I29" s="225" t="s">
         <v>167</v>
@@ -13278,7 +13332,7 @@
       </c>
       <c r="B30" s="120"/>
       <c r="C30" s="129"/>
-      <c r="E30" s="277"/>
+      <c r="E30" s="272"/>
       <c r="F30" s="106"/>
       <c r="I30" s="227" t="s">
         <v>8</v>
@@ -13301,7 +13355,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="126"/>
-      <c r="E31" s="277"/>
+      <c r="E31" s="272"/>
       <c r="F31" s="106"/>
       <c r="I31" s="227" t="s">
         <v>17</v>
@@ -13323,7 +13377,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="126"/>
-      <c r="E32" s="277"/>
+      <c r="E32" s="272"/>
       <c r="F32" s="106"/>
       <c r="I32" s="227" t="s">
         <v>171</v>
@@ -13340,7 +13394,7 @@
       </c>
       <c r="B33" s="121"/>
       <c r="C33" s="129"/>
-      <c r="E33" s="277"/>
+      <c r="E33" s="272"/>
       <c r="F33" s="106"/>
       <c r="I33" s="230" t="s">
         <v>143</v>
@@ -13361,7 +13415,7 @@
       </c>
       <c r="C34" s="126"/>
       <c r="D34" s="108"/>
-      <c r="E34" s="278"/>
+      <c r="E34" s="273"/>
       <c r="F34" s="106"/>
       <c r="L34"/>
     </row>
@@ -13375,7 +13429,7 @@
       </c>
       <c r="C35" s="126"/>
       <c r="D35" s="108"/>
-      <c r="E35" s="277"/>
+      <c r="E35" s="272"/>
       <c r="F35" s="106"/>
       <c r="L35"/>
     </row>
@@ -13388,28 +13442,28 @@
         <v>0</v>
       </c>
       <c r="C36" s="127"/>
-      <c r="E36" s="277"/>
+      <c r="E36" s="272"/>
       <c r="F36" s="106"/>
       <c r="L36"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N37" s="277"/>
+      <c r="N37" s="272"/>
       <c r="O37" s="106"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N38" s="278"/>
+      <c r="N38" s="273"/>
       <c r="O38" s="106"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N39" s="277"/>
+      <c r="N39" s="272"/>
       <c r="O39" s="106"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N40" s="277"/>
+      <c r="N40" s="272"/>
       <c r="O40" s="106"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N41" s="279"/>
+      <c r="N41" s="274"/>
       <c r="O41" s="106"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update home owner city issue
</commit_message>
<xml_diff>
--- a/IntranetPortal/IntranetPortal/App_Data/underwriter.xlsx
+++ b/IntranetPortal/IntranetPortal/App_Data/underwriter.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TasksWebApplication\IntranetPortal\IntranetPortal\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="201">
   <si>
     <t>Property Address:</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>Net Rent</t>
+  </si>
+  <si>
+    <t>Version 1.0</t>
   </si>
 </sst>
 </file>
@@ -2245,6 +2248,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -2266,14 +2277,6 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
@@ -2680,10 +2683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3426,15 +3429,20 @@
       <c r="L32" s="220"/>
       <c r="M32" s="164"/>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D33" s="69"/>
       <c r="E33" s="69"/>
       <c r="F33" s="69"/>
       <c r="G33" s="69"/>
     </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J34" s="147"/>
       <c r="M34" s="147"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="71" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -3549,13 +3557,13 @@
       <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="332">
+      <c r="C2" s="334">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D2" s="332"/>
-      <c r="E2" s="332"/>
-      <c r="F2" s="333"/>
+      <c r="D2" s="334"/>
+      <c r="E2" s="334"/>
+      <c r="F2" s="335"/>
       <c r="G2" s="43"/>
       <c r="H2" s="44" t="s">
         <v>44</v>
@@ -3588,15 +3596,15 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39"/>
-      <c r="B4" s="336" t="s">
+      <c r="B4" s="338" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="337"/>
+      <c r="C4" s="339"/>
       <c r="D4" s="48"/>
-      <c r="E4" s="336" t="s">
+      <c r="E4" s="338" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="337"/>
+      <c r="F4" s="339"/>
       <c r="G4" s="49"/>
       <c r="H4" s="50" t="s">
         <v>42</v>
@@ -3789,13 +3797,13 @@
       <c r="B15" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="332">
+      <c r="C15" s="334">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D15" s="332"/>
-      <c r="E15" s="332"/>
-      <c r="F15" s="333"/>
+      <c r="D15" s="334"/>
+      <c r="E15" s="334"/>
+      <c r="F15" s="335"/>
       <c r="G15" s="43"/>
       <c r="H15" s="138" t="s">
         <v>44</v>
@@ -3828,15 +3836,15 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39"/>
-      <c r="B17" s="334" t="s">
+      <c r="B17" s="336" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="335"/>
+      <c r="C17" s="337"/>
       <c r="D17" s="48"/>
-      <c r="E17" s="334" t="s">
+      <c r="E17" s="336" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="335"/>
+      <c r="F17" s="337"/>
       <c r="G17" s="59"/>
       <c r="H17" s="60" t="s">
         <v>62</v>
@@ -4070,13 +4078,13 @@
       <c r="B30" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="332">
+      <c r="C30" s="334">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D30" s="332"/>
-      <c r="E30" s="332"/>
-      <c r="F30" s="333"/>
+      <c r="D30" s="334"/>
+      <c r="E30" s="334"/>
+      <c r="F30" s="335"/>
       <c r="G30" s="43"/>
       <c r="H30" s="64"/>
       <c r="I30" s="39"/>
@@ -4104,15 +4112,15 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39"/>
-      <c r="B32" s="338" t="s">
+      <c r="B32" s="332" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="339"/>
+      <c r="C32" s="333"/>
       <c r="D32" s="48"/>
-      <c r="E32" s="338" t="s">
+      <c r="E32" s="332" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="339"/>
+      <c r="F32" s="333"/>
       <c r="G32" s="49"/>
       <c r="H32" s="67" t="s">
         <v>40</v>
@@ -4156,15 +4164,15 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="39"/>
-      <c r="B35" s="338" t="s">
+      <c r="B35" s="332" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="339"/>
+      <c r="C35" s="333"/>
       <c r="D35" s="48"/>
-      <c r="E35" s="338" t="s">
+      <c r="E35" s="332" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="339"/>
+      <c r="F35" s="333"/>
       <c r="G35" s="49"/>
       <c r="H35" s="67" t="s">
         <v>54</v>
@@ -4300,17 +4308,17 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="11">
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E32:F32"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="E38:E39">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
@@ -4655,13 +4663,13 @@
       <c r="B11" s="167" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="332">
+      <c r="C11" s="334">
         <f>'Data Input'!C3</f>
         <v>0</v>
       </c>
-      <c r="D11" s="332"/>
-      <c r="E11" s="332"/>
-      <c r="F11" s="333"/>
+      <c r="D11" s="334"/>
+      <c r="E11" s="334"/>
+      <c r="F11" s="335"/>
       <c r="G11" s="39"/>
       <c r="H11" s="148" t="s">
         <v>165</v>

</xml_diff>